<commit_message>
update qtrly monthly numbers
</commit_message>
<xml_diff>
--- a/assets/documents/datasets/Monthly_Numbers_Qrtly.xlsx
+++ b/assets/documents/datasets/Monthly_Numbers_Qrtly.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Website\ONHIRsite\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5AE788-5E8A-45FB-B1A7-CA62837C6F7B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37777311-4EFE-4AF5-945C-C3F216425391}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TABLE A" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="51">
   <si>
     <t>-</t>
   </si>
@@ -177,10 +177,10 @@
     <t>Totals (for all Clients)</t>
   </si>
   <si>
-    <t>Navajo and Hopi Indian Relocation Program Status for DEC, 2019</t>
-  </si>
-  <si>
-    <t>Date of Report  January 1, 2020</t>
+    <t>Date of Report  April 1, 2020</t>
+  </si>
+  <si>
+    <t>Navajo and Hopi Indian Relocation Program Status for Mar, 2020</t>
   </si>
 </sst>
 </file>
@@ -869,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -891,14 +891,14 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -930,7 +930,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="9">
-        <v>3723</v>
+        <v>3724</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>14</v>
@@ -939,13 +939,13 @@
         <v>11</v>
       </c>
       <c r="E5" s="9">
-        <v>3841</v>
+        <v>3842</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>16</v>
       </c>
       <c r="G5" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -953,7 +953,7 @@
         <v>27</v>
       </c>
       <c r="B6" s="9">
-        <v>3211</v>
+        <v>3210</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>18</v>
@@ -962,14 +962,13 @@
         <v>17</v>
       </c>
       <c r="E6" s="9">
-        <v>3343</v>
-      </c>
-      <c r="F6" s="10" t="str">
-        <f>+F7</f>
-        <v>+</v>
+        <v>3342</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>0</v>
       </c>
       <c r="G6" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -1030,7 +1029,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>8</v>
@@ -1039,13 +1038,13 @@
         <v>8</v>
       </c>
       <c r="E10" s="9">
-        <v>3</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>16</v>
+        <v>1</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>0</v>
       </c>
       <c r="G10" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1083,7 +1082,7 @@
         <v>21</v>
       </c>
       <c r="B13" s="10">
-        <v>3723</v>
+        <v>3724</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>14</v>
@@ -1092,13 +1091,13 @@
         <v>11</v>
       </c>
       <c r="E13" s="10">
-        <v>3841</v>
+        <v>3842</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>16</v>
       </c>
       <c r="G13" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -1106,7 +1105,7 @@
         <v>43</v>
       </c>
       <c r="B14" s="10">
-        <v>-3591</v>
+        <v>-3593</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>7</v>
@@ -1115,13 +1114,13 @@
         <v>6</v>
       </c>
       <c r="E14" s="10">
-        <v>-3706</v>
+        <v>-3708</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>16</v>
       </c>
       <c r="G14" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -1152,7 +1151,7 @@
         <v>41</v>
       </c>
       <c r="B16" s="13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>8</v>
@@ -1161,7 +1160,7 @@
         <v>8</v>
       </c>
       <c r="E16" s="13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" s="13" t="s">
         <v>16</v>
@@ -1175,7 +1174,7 @@
         <v>26</v>
       </c>
       <c r="B17" s="13">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>1</v>
@@ -1184,13 +1183,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="13">
-        <v>-3</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>16</v>
+        <v>-1</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>0</v>
       </c>
       <c r="G17" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -1221,7 +1220,7 @@
         <v>44</v>
       </c>
       <c r="B19" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>8</v>
@@ -1230,13 +1229,13 @@
         <v>8</v>
       </c>
       <c r="E19" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F19" s="13" t="s">
         <v>16</v>
       </c>
       <c r="G19" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1274,7 +1273,7 @@
         <v>43</v>
       </c>
       <c r="B22" s="10">
-        <v>3591</v>
+        <v>3593</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>13</v>
@@ -1283,13 +1282,13 @@
         <v>10</v>
       </c>
       <c r="E22" s="10">
-        <v>3706</v>
+        <v>3708</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>16</v>
       </c>
       <c r="G22" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -1297,7 +1296,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="18">
-        <v>-3567</v>
+        <v>-3579</v>
       </c>
       <c r="C23" s="18">
         <v>-88</v>
@@ -1306,13 +1305,13 @@
         <v>-27</v>
       </c>
       <c r="E23" s="18">
-        <v>-3682</v>
+        <v>-3694</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>16</v>
       </c>
       <c r="G23" s="11">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -1320,7 +1319,7 @@
         <v>40</v>
       </c>
       <c r="B24" s="13">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C24" s="13">
         <v>0</v>
@@ -1329,13 +1328,13 @@
         <v>0</v>
       </c>
       <c r="E24" s="13">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>0</v>
       </c>
       <c r="G24" s="14">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -1343,7 +1342,7 @@
         <v>39</v>
       </c>
       <c r="B25" s="20">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>8</v>
@@ -1352,13 +1351,13 @@
         <v>0</v>
       </c>
       <c r="E25" s="20">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G25" s="21">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -1366,7 +1365,7 @@
         <v>28</v>
       </c>
       <c r="B26" s="20">
-        <v>-3208</v>
+        <v>-3209</v>
       </c>
       <c r="C26" s="20">
         <v>-121</v>
@@ -1375,7 +1374,7 @@
         <v>3</v>
       </c>
       <c r="E26" s="20">
-        <v>-3340</v>
+        <v>-3341</v>
       </c>
       <c r="F26" s="20" t="s">
         <v>16</v>

</xml_diff>